<commit_message>
Más recursos por eliminar
Más recursos por eliminar
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion16/escaleta_CN_10_16.xlsx
+++ b/fuentes/contenidos/grado10/guion16/escaleta_CN_10_16.xlsx
@@ -1065,16 +1065,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1116,43 +1153,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1490,9 +1490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,94 +1520,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="60" t="s">
+      <c r="T1" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="52" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="50"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="65"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="59"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1893,123 +1893,123 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+    <row r="9" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="45">
         <v>4</v>
       </c>
-      <c r="I9" s="69" t="s">
+      <c r="I9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="69" t="s">
+      <c r="K9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69" t="s">
+      <c r="M9" s="46"/>
+      <c r="N9" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67" t="s">
+      <c r="O9" s="44"/>
+      <c r="P9" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="67">
+      <c r="Q9" s="44">
         <v>6</v>
       </c>
-      <c r="R9" s="67" t="s">
+      <c r="R9" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S9" s="67" t="s">
+      <c r="S9" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T9" s="67" t="s">
+      <c r="T9" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="U9" s="67" t="s">
+      <c r="U9" s="44" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+    <row r="10" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67" t="s">
+      <c r="F10" s="44"/>
+      <c r="G10" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="45">
         <v>5</v>
       </c>
-      <c r="I10" s="69" t="s">
+      <c r="I10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="69" t="s">
+      <c r="K10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="69" t="s">
+      <c r="L10" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="69" t="s">
+      <c r="M10" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67" t="s">
+      <c r="N10" s="46"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="67">
+      <c r="Q10" s="44">
         <v>6</v>
       </c>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="S10" s="67" t="s">
+      <c r="S10" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="T10" s="67" t="s">
+      <c r="T10" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="U10" s="67" t="s">
+      <c r="U10" s="44" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2190,62 +2190,62 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="44"/>
+      <c r="G14" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="45">
         <v>9</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8" t="s">
+      <c r="M14" s="46"/>
+      <c r="N14" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34" t="s">
+      <c r="O14" s="49"/>
+      <c r="P14" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="44">
         <v>6</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S14" s="10" t="s">
+      <c r="S14" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T14" s="12" t="s">
+      <c r="T14" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="U14" s="10" t="s">
+      <c r="U14" s="44" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2431,62 +2431,62 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+    <row r="19" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="67" t="s">
+      <c r="D19" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67" t="s">
+      <c r="F19" s="44"/>
+      <c r="G19" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="45">
         <v>12</v>
       </c>
-      <c r="I19" s="69" t="s">
+      <c r="I19" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="67" t="s">
+      <c r="J19" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="K19" s="69" t="s">
+      <c r="K19" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="69" t="s">
+      <c r="L19" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69" t="s">
+      <c r="M19" s="46"/>
+      <c r="N19" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="O19" s="67"/>
-      <c r="P19" s="67" t="s">
+      <c r="O19" s="44"/>
+      <c r="P19" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="67">
+      <c r="Q19" s="44">
         <v>6</v>
       </c>
-      <c r="R19" s="67" t="s">
+      <c r="R19" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S19" s="67" t="s">
+      <c r="S19" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T19" s="67" t="s">
+      <c r="T19" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="U19" s="67" t="s">
+      <c r="U19" s="44" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2641,239 +2641,239 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+    <row r="23" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="67" t="s">
+      <c r="D23" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E23" s="67" t="s">
+      <c r="E23" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67" t="s">
+      <c r="F23" s="44"/>
+      <c r="G23" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="45">
         <v>15</v>
       </c>
-      <c r="I23" s="69" t="s">
+      <c r="I23" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="67" t="s">
+      <c r="J23" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="K23" s="69" t="s">
+      <c r="K23" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="69" t="s">
+      <c r="L23" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M23" s="69" t="s">
+      <c r="M23" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="69"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67" t="s">
+      <c r="N23" s="46"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="70">
+      <c r="Q23" s="47">
         <v>6</v>
       </c>
-      <c r="R23" s="70" t="s">
+      <c r="R23" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="S23" s="70" t="s">
+      <c r="S23" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="T23" s="71" t="s">
+      <c r="T23" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="U23" s="70" t="s">
+      <c r="U23" s="47" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="16" t="s">
+      <c r="F24" s="44"/>
+      <c r="G24" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="45">
         <v>16</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8" t="s">
+      <c r="M24" s="46"/>
+      <c r="N24" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9" t="s">
+      <c r="O24" s="44"/>
+      <c r="P24" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="Q24" s="44">
         <v>6</v>
       </c>
-      <c r="R24" s="11" t="s">
+      <c r="R24" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S24" s="10" t="s">
+      <c r="S24" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T24" s="12" t="s">
+      <c r="T24" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="44" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="16" t="s">
+      <c r="F25" s="44"/>
+      <c r="G25" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="H25" s="39">
+      <c r="H25" s="45">
         <v>17</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8" t="s">
+      <c r="M25" s="46"/>
+      <c r="N25" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9" t="s">
+      <c r="O25" s="44"/>
+      <c r="P25" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q25" s="44">
         <v>6</v>
       </c>
-      <c r="R25" s="11" t="s">
+      <c r="R25" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S25" s="10" t="s">
+      <c r="S25" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T25" s="12" t="s">
+      <c r="T25" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="U25" s="10" t="s">
+      <c r="U25" s="44" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="16" t="s">
+      <c r="F26" s="44"/>
+      <c r="G26" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="45">
         <v>18</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8" t="s">
+      <c r="M26" s="46"/>
+      <c r="N26" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9" t="s">
+      <c r="O26" s="44"/>
+      <c r="P26" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="44">
         <v>6</v>
       </c>
-      <c r="R26" s="11" t="s">
+      <c r="R26" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S26" s="10" t="s">
+      <c r="S26" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T26" s="12" t="s">
+      <c r="T26" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="U26" s="10" t="s">
+      <c r="U26" s="44" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2997,62 +2997,62 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="64" t="s">
+    <row r="29" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="67" t="s">
+      <c r="D29" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E29" s="67" t="s">
+      <c r="E29" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67" t="s">
+      <c r="F29" s="44"/>
+      <c r="G29" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="H29" s="68">
+      <c r="H29" s="45">
         <v>21</v>
       </c>
-      <c r="I29" s="69" t="s">
+      <c r="I29" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="67" t="s">
+      <c r="J29" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="K29" s="69" t="s">
+      <c r="K29" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="69" t="s">
+      <c r="L29" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69" t="s">
+      <c r="M29" s="46"/>
+      <c r="N29" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="67"/>
-      <c r="P29" s="67" t="s">
+      <c r="O29" s="44"/>
+      <c r="P29" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="67">
+      <c r="Q29" s="44">
         <v>6</v>
       </c>
-      <c r="R29" s="67" t="s">
+      <c r="R29" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S29" s="67" t="s">
+      <c r="S29" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T29" s="67" t="s">
+      <c r="T29" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="U29" s="67" t="s">
+      <c r="U29" s="44" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3115,117 +3115,117 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="64" t="s">
+    <row r="31" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="67" t="s">
+      <c r="D31" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67" t="s">
+      <c r="E31" s="13"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="H31" s="68">
+      <c r="H31" s="39">
         <v>23</v>
       </c>
-      <c r="I31" s="69" t="s">
+      <c r="I31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="67" t="s">
+      <c r="J31" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="K31" s="69" t="s">
+      <c r="K31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="69" t="s">
+      <c r="L31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69" t="s">
+      <c r="M31" s="8"/>
+      <c r="N31" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67" t="s">
+      <c r="O31" s="9"/>
+      <c r="P31" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="67">
+      <c r="Q31" s="10">
         <v>6</v>
       </c>
-      <c r="R31" s="67" t="s">
+      <c r="R31" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="S31" s="67" t="s">
+      <c r="S31" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="T31" s="67" t="s">
+      <c r="T31" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="U31" s="67" t="s">
+      <c r="U31" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="16" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="45">
         <v>24</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K32" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8" t="s">
+      <c r="M32" s="46"/>
+      <c r="N32" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9" t="s">
+      <c r="O32" s="44"/>
+      <c r="P32" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="10">
+      <c r="Q32" s="44">
         <v>6</v>
       </c>
-      <c r="R32" s="11" t="s">
+      <c r="R32" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="S32" s="10" t="s">
+      <c r="S32" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="T32" s="12" t="s">
+      <c r="T32" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="U32" s="10" t="s">
+      <c r="U32" s="44" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4671,12 +4671,6 @@
     <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4691,6 +4685,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>

</xml_diff>

<commit_message>
Eliminación de recurso 11_16
Eliminación de recurso 11_16
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion16/escaleta_CN_10_16.xlsx
+++ b/fuentes/contenidos/grado10/guion16/escaleta_CN_10_16.xlsx
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$35</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -839,7 +839,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,6 +930,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -987,7 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1060,7 +1066,6 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1096,16 +1101,49 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1147,39 +1185,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1187,6 +1207,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1517,9 +1542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,94 +1572,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="76"/>
+      <c r="O1" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="67" t="s">
+      <c r="S1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="67" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="71"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="68"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="59"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1664,7 +1689,7 @@
       <c r="I3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>127</v>
       </c>
       <c r="K3" s="22" t="s">
@@ -1717,7 +1742,7 @@
       <c r="G4" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="38">
         <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -1776,7 +1801,7 @@
         <v>133</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="39"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="5"/>
       <c r="J5" s="17"/>
       <c r="K5" s="7"/>
@@ -1811,7 +1836,7 @@
         <v>134</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="5"/>
       <c r="J6" s="17"/>
       <c r="K6" s="7"/>
@@ -1844,7 +1869,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="39"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="5"/>
       <c r="J7" s="17"/>
       <c r="K7" s="7"/>
@@ -1881,7 +1906,7 @@
       <c r="G8" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="38">
         <v>3</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1920,123 +1945,123 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="44">
         <v>4</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="K9" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="L9" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46" t="s">
+      <c r="M9" s="45"/>
+      <c r="N9" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44" t="s">
+      <c r="O9" s="43"/>
+      <c r="P9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="44">
+      <c r="Q9" s="43">
         <v>6</v>
       </c>
-      <c r="R9" s="44" t="s">
+      <c r="R9" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S9" s="44" t="s">
+      <c r="S9" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T9" s="44" t="s">
+      <c r="T9" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="U9" s="44" t="s">
+      <c r="U9" s="43" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+    <row r="10" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="44">
         <v>5</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="K10" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="46" t="s">
+      <c r="M10" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="46"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44" t="s">
+      <c r="N10" s="45"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="44">
+      <c r="Q10" s="43">
         <v>6</v>
       </c>
-      <c r="R10" s="44" t="s">
+      <c r="R10" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="S10" s="44" t="s">
+      <c r="S10" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="T10" s="44" t="s">
+      <c r="T10" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="U10" s="44" t="s">
+      <c r="U10" s="43" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2060,7 +2085,7 @@
       <c r="G11" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="38">
         <v>6</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -2158,121 +2183,121 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:21" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="81"/>
+      <c r="G13" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="82">
         <v>8</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34" t="s">
+      <c r="N13" s="83"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="81">
         <v>6</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="S13" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="T13" s="12" t="s">
+      <c r="T13" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="U13" s="10" t="s">
+      <c r="U13" s="81" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44" t="s">
+      <c r="F14" s="43"/>
+      <c r="G14" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="H14" s="45">
+      <c r="H14" s="44">
         <v>9</v>
       </c>
-      <c r="I14" s="46" t="s">
+      <c r="I14" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="K14" s="46" t="s">
+      <c r="K14" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="46" t="s">
+      <c r="L14" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46" t="s">
+      <c r="M14" s="45"/>
+      <c r="N14" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49" t="s">
+      <c r="O14" s="48"/>
+      <c r="P14" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="44">
+      <c r="Q14" s="43">
         <v>6</v>
       </c>
-      <c r="R14" s="44" t="s">
+      <c r="R14" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S14" s="44" t="s">
+      <c r="S14" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T14" s="44" t="s">
+      <c r="T14" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="U14" s="44" t="s">
+      <c r="U14" s="43" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2327,7 +2352,7 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="39"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="5"/>
       <c r="J16" s="17"/>
       <c r="K16" s="7"/>
@@ -2362,7 +2387,7 @@
       <c r="G17" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="38">
         <v>10</v>
       </c>
       <c r="I17" s="5" t="s">
@@ -2421,7 +2446,7 @@
       <c r="G18" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="38">
         <v>11</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -2458,62 +2483,62 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44" t="s">
+      <c r="F19" s="43"/>
+      <c r="G19" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="44">
         <v>12</v>
       </c>
-      <c r="I19" s="46" t="s">
+      <c r="I19" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="46" t="s">
+      <c r="L19" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46" t="s">
+      <c r="M19" s="45"/>
+      <c r="N19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44" t="s">
+      <c r="O19" s="43"/>
+      <c r="P19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="44">
+      <c r="Q19" s="43">
         <v>6</v>
       </c>
-      <c r="R19" s="44" t="s">
+      <c r="R19" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S19" s="44" t="s">
+      <c r="S19" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T19" s="44" t="s">
+      <c r="T19" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="U19" s="44" t="s">
+      <c r="U19" s="43" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2629,7 +2654,7 @@
       <c r="G22" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="38">
         <v>14</v>
       </c>
       <c r="I22" s="5" t="s">
@@ -2646,7 +2671,7 @@
       </c>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
-      <c r="O22" s="40" t="s">
+      <c r="O22" s="39" t="s">
         <v>243</v>
       </c>
       <c r="P22" s="9" t="s">
@@ -2668,298 +2693,298 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+    <row r="23" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44" t="s">
+      <c r="F23" s="43"/>
+      <c r="G23" s="43" t="s">
         <v>241</v>
       </c>
-      <c r="H23" s="45">
+      <c r="H23" s="44">
         <v>15</v>
       </c>
-      <c r="I23" s="46" t="s">
+      <c r="I23" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="K23" s="46" t="s">
+      <c r="K23" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="M23" s="46" t="s">
+      <c r="M23" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="46"/>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44" t="s">
+      <c r="N23" s="45"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="47">
+      <c r="Q23" s="46">
         <v>6</v>
       </c>
-      <c r="R23" s="47" t="s">
+      <c r="R23" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="S23" s="47" t="s">
+      <c r="S23" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="T23" s="48" t="s">
+      <c r="T23" s="47" t="s">
         <v>244</v>
       </c>
-      <c r="U23" s="47" t="s">
+      <c r="U23" s="46" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44" t="s">
+      <c r="F24" s="43"/>
+      <c r="G24" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="H24" s="45">
+      <c r="H24" s="44">
         <v>16</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="44" t="s">
+      <c r="J24" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="K24" s="46" t="s">
+      <c r="K24" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46" t="s">
+      <c r="M24" s="45"/>
+      <c r="N24" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44" t="s">
+      <c r="O24" s="43"/>
+      <c r="P24" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="44">
+      <c r="Q24" s="43">
         <v>6</v>
       </c>
-      <c r="R24" s="44" t="s">
+      <c r="R24" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S24" s="44" t="s">
+      <c r="S24" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T24" s="44" t="s">
+      <c r="T24" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="U24" s="44" t="s">
+      <c r="U24" s="43" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44" t="s">
+      <c r="F25" s="43"/>
+      <c r="G25" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="H25" s="45">
+      <c r="H25" s="44">
         <v>17</v>
       </c>
-      <c r="I25" s="46" t="s">
+      <c r="I25" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="44" t="s">
+      <c r="J25" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="K25" s="46" t="s">
+      <c r="K25" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="46" t="s">
+      <c r="L25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46" t="s">
+      <c r="M25" s="45"/>
+      <c r="N25" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44" t="s">
+      <c r="O25" s="43"/>
+      <c r="P25" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="44">
+      <c r="Q25" s="43">
         <v>6</v>
       </c>
-      <c r="R25" s="44" t="s">
+      <c r="R25" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S25" s="44" t="s">
+      <c r="S25" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T25" s="44" t="s">
+      <c r="T25" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="U25" s="44" t="s">
+      <c r="U25" s="43" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44" t="s">
+      <c r="F26" s="43"/>
+      <c r="G26" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="H26" s="45">
+      <c r="H26" s="44">
         <v>18</v>
       </c>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="46" t="s">
+      <c r="K26" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46" t="s">
+      <c r="M26" s="45"/>
+      <c r="N26" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44" t="s">
+      <c r="O26" s="43"/>
+      <c r="P26" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="44">
+      <c r="Q26" s="43">
         <v>6</v>
       </c>
-      <c r="R26" s="44" t="s">
+      <c r="R26" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S26" s="44" t="s">
+      <c r="S26" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T26" s="44" t="s">
+      <c r="T26" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="U26" s="44" t="s">
+      <c r="U26" s="43" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44" t="s">
+      <c r="F27" s="43"/>
+      <c r="G27" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="H27" s="45">
+      <c r="H27" s="44">
         <v>19</v>
       </c>
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="44" t="s">
+      <c r="J27" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="K27" s="46" t="s">
+      <c r="K27" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="46" t="s">
+      <c r="L27" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46" t="s">
+      <c r="M27" s="45"/>
+      <c r="N27" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44" t="s">
+      <c r="O27" s="43"/>
+      <c r="P27" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="44">
+      <c r="Q27" s="43">
         <v>6</v>
       </c>
-      <c r="R27" s="44" t="s">
+      <c r="R27" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S27" s="44" t="s">
+      <c r="S27" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T27" s="44" t="s">
+      <c r="T27" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="U27" s="44" t="s">
+      <c r="U27" s="43" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2983,7 +3008,7 @@
       <c r="G28" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="38">
         <v>20</v>
       </c>
       <c r="I28" s="5" t="s">
@@ -3024,62 +3049,62 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="79" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="75" t="s">
+    <row r="29" spans="1:21" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="73" t="s">
+      <c r="D29" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73" t="s">
+      <c r="F29" s="49"/>
+      <c r="G29" s="49" t="s">
         <v>223</v>
       </c>
-      <c r="H29" s="77">
+      <c r="H29" s="53">
         <v>21</v>
       </c>
-      <c r="I29" s="78" t="s">
+      <c r="I29" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="73" t="s">
+      <c r="J29" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="K29" s="78" t="s">
+      <c r="K29" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="78" t="s">
+      <c r="L29" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78" t="s">
+      <c r="M29" s="54"/>
+      <c r="N29" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="73"/>
-      <c r="P29" s="74" t="s">
+      <c r="O29" s="49"/>
+      <c r="P29" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="73">
+      <c r="Q29" s="49">
         <v>6</v>
       </c>
-      <c r="R29" s="73" t="s">
+      <c r="R29" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="S29" s="73" t="s">
+      <c r="S29" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="T29" s="73" t="s">
+      <c r="T29" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="U29" s="73" t="s">
+      <c r="U29" s="49" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3103,7 +3128,7 @@
       <c r="G30" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="38">
         <v>22</v>
       </c>
       <c r="I30" s="5" t="s">
@@ -3142,7 +3167,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>17</v>
       </c>
@@ -3160,7 +3185,7 @@
       <c r="G31" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="H31" s="39">
+      <c r="H31" s="38">
         <v>23</v>
       </c>
       <c r="I31" s="5" t="s">
@@ -3200,59 +3225,59 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44" t="s">
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="44">
         <v>24</v>
       </c>
-      <c r="I32" s="46" t="s">
+      <c r="I32" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="44" t="s">
+      <c r="J32" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="K32" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="46" t="s">
+      <c r="L32" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46" t="s">
+      <c r="M32" s="45"/>
+      <c r="N32" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44" t="s">
+      <c r="O32" s="43"/>
+      <c r="P32" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="44">
+      <c r="Q32" s="43">
         <v>6</v>
       </c>
-      <c r="R32" s="44" t="s">
+      <c r="R32" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="S32" s="44" t="s">
+      <c r="S32" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="T32" s="44" t="s">
+      <c r="T32" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="U32" s="44" t="s">
+      <c r="U32" s="43" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3274,7 +3299,7 @@
       <c r="G33" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="38">
         <v>25</v>
       </c>
       <c r="I33" s="5" t="s">
@@ -3319,13 +3344,13 @@
       <c r="G34" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="39">
+      <c r="H34" s="38">
         <v>26</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="36" t="s">
+      <c r="J34" s="35" t="s">
         <v>186</v>
       </c>
       <c r="K34" s="7" t="s">
@@ -3373,16 +3398,16 @@
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="H35" s="39">
+      <c r="H35" s="38">
         <v>27</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="38" t="s">
+      <c r="J35" s="37" t="s">
         <v>185</v>
       </c>
       <c r="K35" s="7" t="s">
@@ -4698,12 +4723,6 @@
     <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4718,6 +4737,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>

</xml_diff>